<commit_message>
Projectile comms pins added
 - Projectile comms pins defaulted to SPI.
- Some pins may change due to PWM output needing to be on TCxWO[1] pin.
- Projectile fitted feedback connected via internal pull down.
</commit_message>
<xml_diff>
--- a/OWE003827-SkyWall300-Launcher-Firmware/Diagrams/OWE003827_v0_PinMap.xlsx
+++ b/OWE003827-SkyWall300-Launcher-Firmware/Diagrams/OWE003827_v0_PinMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Fitzgerald\Documents\GitHub\OWE003827-SkyWall300-Launcher-Firmware\OWE003827-SkyWall300-Launcher-Firmware\Diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCEB28D-12B6-4B42-9DD0-6FA87D04115C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677253AC-D0CB-42EF-A72E-81BB27AA6A05}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{D4CCC71D-D02E-4408-870A-1445D0B22066}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="59">
   <si>
     <t>Pin Name</t>
   </si>
@@ -154,6 +154,54 @@
   </si>
   <si>
     <t>PB25</t>
+  </si>
+  <si>
+    <t>PROJECTILE_MOSI</t>
+  </si>
+  <si>
+    <t>PA23</t>
+  </si>
+  <si>
+    <t>SERCOM5 PAD0</t>
+  </si>
+  <si>
+    <t>SPI ASYNC</t>
+  </si>
+  <si>
+    <t>PROJECTILE_SCK</t>
+  </si>
+  <si>
+    <t>PA22</t>
+  </si>
+  <si>
+    <t>SERCOM5 PAD1</t>
+  </si>
+  <si>
+    <t>MOSI</t>
+  </si>
+  <si>
+    <t>SCK</t>
+  </si>
+  <si>
+    <t>PROJECTILE_MISO</t>
+  </si>
+  <si>
+    <t>PA21</t>
+  </si>
+  <si>
+    <t>MISO</t>
+  </si>
+  <si>
+    <t>SERCOM5 PAD3</t>
+  </si>
+  <si>
+    <t>PROJECTILE_FITTED_FB</t>
+  </si>
+  <si>
+    <t>PA20</t>
+  </si>
+  <si>
+    <t>GPIO in, pull down.</t>
   </si>
 </sst>
 </file>
@@ -531,15 +579,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{639EB9ED-E079-47B5-B490-1C21FC73A212}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="17.7109375" style="2"/>
+    <col min="1" max="1" width="30.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="17.7109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -740,6 +794,68 @@
       </c>
       <c r="C15" s="2" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
System pressure and charge enable feedback signals added
- Internally pulled high (pressure and charge enable disabled)
</commit_message>
<xml_diff>
--- a/OWE003827-SkyWall300-Launcher-Firmware/Diagrams/OWE003827_v0_PinMap.xlsx
+++ b/OWE003827-SkyWall300-Launcher-Firmware/Diagrams/OWE003827_v0_PinMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Fitzgerald\Documents\GitHub\OWE003827-SkyWall300-Launcher-Firmware\OWE003827-SkyWall300-Launcher-Firmware\Diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677253AC-D0CB-42EF-A72E-81BB27AA6A05}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E8CA49-70B7-41EC-AF2D-2744F5C61A66}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{D4CCC71D-D02E-4408-870A-1445D0B22066}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="73">
   <si>
     <t>Pin Name</t>
   </si>
@@ -202,6 +202,48 @@
   </si>
   <si>
     <t>GPIO in, pull down.</t>
+  </si>
+  <si>
+    <t>PROJECTILE_COMMS_ENABLE_OP</t>
+  </si>
+  <si>
+    <t>PB21</t>
+  </si>
+  <si>
+    <t>FILL_VALVE_COARSE_OP</t>
+  </si>
+  <si>
+    <t>PB17</t>
+  </si>
+  <si>
+    <t>PB16</t>
+  </si>
+  <si>
+    <t>PD21</t>
+  </si>
+  <si>
+    <t>PD20</t>
+  </si>
+  <si>
+    <t>FILL_VALVE_FINE_OP</t>
+  </si>
+  <si>
+    <t>DUMP_VALVE_COARSE_OP</t>
+  </si>
+  <si>
+    <t>DUMP_VALVE_FINE_OP</t>
+  </si>
+  <si>
+    <t>SYSTEM_CHARGE_ENABLE_FB</t>
+  </si>
+  <si>
+    <t>PC23</t>
+  </si>
+  <si>
+    <t>SYSTEM_PRESSURE_ENABLE_FB</t>
+  </si>
+  <si>
+    <t>PC22</t>
   </si>
 </sst>
 </file>
@@ -579,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{639EB9ED-E079-47B5-B490-1C21FC73A212}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,6 +900,83 @@
         <v>58</v>
       </c>
     </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:D1"/>

</xml_diff>

<commit_message>
Added checks for motor feedback
</commit_message>
<xml_diff>
--- a/OWE003827-SkyWall300-Launcher-Firmware/Diagrams/OWE003827_v0_PinMap.xlsx
+++ b/OWE003827-SkyWall300-Launcher-Firmware/Diagrams/OWE003827_v0_PinMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Fitzgerald\Documents\GitHub\OWE003827-SkyWall300-Launcher-Firmware\OWE003827-SkyWall300-Launcher-Firmware\Diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E8CA49-70B7-41EC-AF2D-2744F5C61A66}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FEA4FA-5090-44D4-90A8-F37A2F59768D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{D4CCC71D-D02E-4408-870A-1445D0B22066}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="79">
   <si>
     <t>Pin Name</t>
   </si>
@@ -244,6 +244,24 @@
   </si>
   <si>
     <t>PC22</t>
+  </si>
+  <si>
+    <t>PB13</t>
+  </si>
+  <si>
+    <t>PB12</t>
+  </si>
+  <si>
+    <t>DIAG_COMMS_RX</t>
+  </si>
+  <si>
+    <t>DIAG_COMMS_TX</t>
+  </si>
+  <si>
+    <t>SERCOM4 PAD1</t>
+  </si>
+  <si>
+    <t>SERCOM4 PAD0</t>
   </si>
 </sst>
 </file>
@@ -621,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{639EB9ED-E079-47B5-B490-1C21FC73A212}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,6 +995,46 @@
         <v>4</v>
       </c>
     </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:D1"/>

</xml_diff>

<commit_message>
Error and Status LEDs added. DAC output added. ADC inputs added.
- DAC voltage reference set to buffered external.
- All ADC inputs are on ADC1, 12 bits.
</commit_message>
<xml_diff>
--- a/OWE003827-SkyWall300-Launcher-Firmware/Diagrams/OWE003827_v0_PinMap.xlsx
+++ b/OWE003827-SkyWall300-Launcher-Firmware/Diagrams/OWE003827_v0_PinMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Fitzgerald\Documents\GitHub\OWE003827-SkyWall300-Launcher-Firmware\OWE003827-SkyWall300-Launcher-Firmware\Diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FEA4FA-5090-44D4-90A8-F37A2F59768D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC9FD80-7092-471C-98DF-05D9C65A0FB0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{D4CCC71D-D02E-4408-870A-1445D0B22066}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="117">
   <si>
     <t>Pin Name</t>
   </si>
@@ -262,6 +262,120 @@
   </si>
   <si>
     <t>SERCOM4 PAD0</t>
+  </si>
+  <si>
+    <t>PROJECTILE_VOLTAGE_FB</t>
+  </si>
+  <si>
+    <t>QSPI</t>
+  </si>
+  <si>
+    <t>PC06</t>
+  </si>
+  <si>
+    <t>PC05</t>
+  </si>
+  <si>
+    <t>PROJECTILE_CURRENT_FB</t>
+  </si>
+  <si>
+    <t>PB11</t>
+  </si>
+  <si>
+    <t>PB10</t>
+  </si>
+  <si>
+    <t>PA11</t>
+  </si>
+  <si>
+    <t>PA10</t>
+  </si>
+  <si>
+    <t>PA09</t>
+  </si>
+  <si>
+    <t>PA08</t>
+  </si>
+  <si>
+    <t>PA07</t>
+  </si>
+  <si>
+    <t>STATUS_LED_OP</t>
+  </si>
+  <si>
+    <t>PA06</t>
+  </si>
+  <si>
+    <t>ERROR_LED_OP</t>
+  </si>
+  <si>
+    <t>PA05</t>
+  </si>
+  <si>
+    <t>DAC</t>
+  </si>
+  <si>
+    <t>VOUT1</t>
+  </si>
+  <si>
+    <t>VOUT0</t>
+  </si>
+  <si>
+    <t>ADC IN</t>
+  </si>
+  <si>
+    <t>ADC1 1</t>
+  </si>
+  <si>
+    <t>PB09</t>
+  </si>
+  <si>
+    <t>PROJECTILE_CHARGE_CURRENT_AN</t>
+  </si>
+  <si>
+    <t>PROJECTILE_CHARGE_VOLTAGE_AN</t>
+  </si>
+  <si>
+    <t>PB08</t>
+  </si>
+  <si>
+    <t>ADC1 0</t>
+  </si>
+  <si>
+    <t>RES_PRESSURE_B_AN</t>
+  </si>
+  <si>
+    <t>PD00</t>
+  </si>
+  <si>
+    <t>ADC1 14</t>
+  </si>
+  <si>
+    <t>RES_PRESSURE_A_AN</t>
+  </si>
+  <si>
+    <t>PB05</t>
+  </si>
+  <si>
+    <t>ADC1 7</t>
+  </si>
+  <si>
+    <t>HW_VERSION_AN</t>
+  </si>
+  <si>
+    <t>PB04</t>
+  </si>
+  <si>
+    <t>ADC1 6</t>
+  </si>
+  <si>
+    <t>PA02</t>
+  </si>
+  <si>
+    <t>PROJECTILE_CHARGE_CURRENT_AO</t>
+  </si>
+  <si>
+    <t>PROJECTILE_CHARGE_VOLTAGE_AO</t>
   </si>
 </sst>
 </file>
@@ -639,15 +753,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{639EB9ED-E079-47B5-B490-1C21FC73A212}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
@@ -1035,6 +1149,196 @@
         <v>11</v>
       </c>
     </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:D1"/>

</xml_diff>